<commit_message>
Done with sections 9-1 and 9-2 :)
</commit_message>
<xml_diff>
--- a/Documentación/Tablas/9-1 Diseño de banco de pruebas.xlsx
+++ b/Documentación/Tablas/9-1 Diseño de banco de pruebas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CABC03F-FA02-4C6E-82A9-1FE0CB63B7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F274B9B3-9F19-459F-AF18-7B0E0ED2A5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Banco</t>
   </si>
@@ -54,39 +54,40 @@
     <t>BP-05</t>
   </si>
   <si>
-    <t>Penguin Logger.
-Penguin Base.
-Data Logger de alimentacíon.
-Fuente regulada de 5V, capaz de entregar al menos 100mA.
-Sensor de temperatura calibrado.
-Cronómetro calibrado.
-Recipiente con agua salada.</t>
-  </si>
-  <si>
-    <t>Penguin Logger.
-Batería utilizada.
-Data Logger.</t>
-  </si>
-  <si>
-    <t>Penguin Logger, sellado en su poteo.
-Penguin Base.
-Instrumentos de medición dimensional con resolución de al menos 1mm.
-Balanza digital con resolución de al menos 0.1g</t>
-  </si>
-  <si>
-    <t>Penguin Logger, sellado en su poteo.
-Penguin Base.
-Cámara de presión calibrada, capaz de generar al menos 10bar de presión.
-Sensor de temperatura calibrado.
-Recipiente con agua salada</t>
-  </si>
-  <si>
-    <t>Penguin Logger, sellado en su poteo y con datos.
-Penguin Base.
-Computadora con programa de recoleccíon de datos (PenGUI).</t>
-  </si>
-  <si>
-    <t>Ver "Plan de validacion" de "Sistema de Monitoreo de Fauna Silvestre"</t>
+    <t>FOTO</t>
+  </si>
+  <si>
+    <t>\tabitem Penguin Logger.
+\tabitem Penguin Base.
+\tabitem Data Logger de alimentacíon.
+\tabitem Fuente regulada de 3.3V, capaz de entregar al menos 100mA.
+\tabitem Sensor de temperatura calibrado.
+\tabitem Cronómetro calibrado.
+\tabitem Recipiente con agua salada.</t>
+  </si>
+  <si>
+    <t>\tabitem Penguin Logger.
+\tabitem Batería utilizada.
+\tabitem Data Logger.</t>
+  </si>
+  <si>
+    <t>\tabitem Penguin Logger, sellado en su poteo.
+\tabitem Penguin Base.
+\tabitem Instrumentos de medición dimensional con resolución de al menos 1mm.
+\tabitem Balanza digital con resolución de al menos 0.1g.</t>
+  </si>
+  <si>
+    <t>\tabitem Penguin Logger, sellado en su poteo.
+\tabitem Penguin Base.
+\tabitem Cámara de presión calibrada, capaz de generar al menos 10bar de presión.
+\tabitem Manómetro calibrado.
+\tabitem Sensor de temperatura calibrado.
+\tabitem Recipiente con agua salada.</t>
+  </si>
+  <si>
+    <t>\tabitem Penguin Logger, sellado en su poteo y con datos.
+\tabitem Penguin Base.
+\tabitem Computadora con programa de recoleccíon de datos (PenGUI).</t>
   </si>
 </sst>
 </file>
@@ -137,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -160,20 +161,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -465,66 +540,82 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="73.5703125" customWidth="1"/>
+    <col min="3" max="3" width="73.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>